<commit_message>
Reorganizing R folder to improve clarity of workflow
</commit_message>
<xml_diff>
--- a/AquaticMacroInvert_metadata.xlsx
+++ b/AquaticMacroInvert_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\aquatic_data\git\EuroAquaticMacroInverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ABBE0D-C829-41A5-97A7-8158653009C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985DBFA5-A996-448C-B96D-A950372A882B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="348" windowWidth="13776" windowHeight="11736" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9156" yWindow="1416" windowWidth="14436" windowHeight="11724" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="5" r:id="rId1"/>
@@ -9128,9 +9128,6 @@
     <t>elevation_atPoint</t>
   </si>
   <si>
-    <t>slope_atPoint</t>
-  </si>
-  <si>
     <t>dam_impact_score_lessthan100km</t>
   </si>
   <si>
@@ -9222,9 +9219,6 @@
   </si>
   <si>
     <t>elevation at site location (m)</t>
-  </si>
-  <si>
-    <t>slope (downstream elevation difference divided by distance) at site location (%)</t>
   </si>
   <si>
     <t>cropland within the microbasin site is located within (%), average of the years 1992-2018 which overlap with sampling period (e.g. for a site with sampling from 1990-2010, this is the average of values from 1992-2010).</t>
@@ -9528,6 +9522,12 @@
   </si>
   <si>
     <t>functional redundancy</t>
+  </si>
+  <si>
+    <t>slope_mean</t>
+  </si>
+  <si>
+    <t>mean slope (downstream elevation difference divided by distance) within microbasin site is located (%)</t>
   </si>
 </sst>
 </file>
@@ -103434,7 +103434,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -103443,15 +103445,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3154</v>
+        <v>3152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>3035</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3036</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3037</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -103459,15 +103461,15 @@
         <v>3017</v>
       </c>
       <c r="B4" t="s">
-        <v>3038</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3118</v>
+        <v>3116</v>
       </c>
       <c r="B5" t="s">
-        <v>3124</v>
+        <v>3122</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -103475,7 +103477,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>3039</v>
+        <v>3038</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -103483,7 +103485,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>3040</v>
+        <v>3039</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -103491,7 +103493,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>3041</v>
+        <v>3040</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -103499,7 +103501,7 @@
         <v>2788</v>
       </c>
       <c r="B9" t="s">
-        <v>3042</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -103507,7 +103509,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>3043</v>
+        <v>3042</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -103515,7 +103517,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>3044</v>
+        <v>3043</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -103523,7 +103525,7 @@
         <v>3018</v>
       </c>
       <c r="B12" t="s">
-        <v>3045</v>
+        <v>3044</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -103531,7 +103533,7 @@
         <v>3019</v>
       </c>
       <c r="B13" t="s">
-        <v>3046</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -103539,7 +103541,7 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>3047</v>
+        <v>3046</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -103547,7 +103549,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>3048</v>
+        <v>3047</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -103555,7 +103557,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>3049</v>
+        <v>3048</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -103563,7 +103565,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>3050</v>
+        <v>3049</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -103571,7 +103573,7 @@
         <v>2779</v>
       </c>
       <c r="B18" t="s">
-        <v>3051</v>
+        <v>3050</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -103579,7 +103581,7 @@
         <v>2780</v>
       </c>
       <c r="B19" t="s">
-        <v>3052</v>
+        <v>3051</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -103587,7 +103589,7 @@
         <v>2781</v>
       </c>
       <c r="B20" t="s">
-        <v>3053</v>
+        <v>3052</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -103595,39 +103597,39 @@
         <v>3020</v>
       </c>
       <c r="B21" t="s">
-        <v>3054</v>
+        <v>3053</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>3104</v>
+        <v>3102</v>
       </c>
       <c r="B22" t="s">
-        <v>3108</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>3105</v>
+        <v>3103</v>
       </c>
       <c r="B23" t="s">
-        <v>3109</v>
+        <v>3107</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>3106</v>
+        <v>3104</v>
       </c>
       <c r="B24" t="s">
-        <v>3110</v>
+        <v>3108</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>3107</v>
+        <v>3105</v>
       </c>
       <c r="B25" t="s">
-        <v>3111</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -103635,7 +103637,7 @@
         <v>3021</v>
       </c>
       <c r="B26" t="s">
-        <v>3055</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -103643,7 +103645,7 @@
         <v>3022</v>
       </c>
       <c r="B27" t="s">
-        <v>3056</v>
+        <v>3055</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -103651,15 +103653,15 @@
         <v>3023</v>
       </c>
       <c r="B28" t="s">
-        <v>3057</v>
+        <v>3056</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>3112</v>
+        <v>3110</v>
       </c>
       <c r="B29" t="s">
-        <v>3113</v>
+        <v>3111</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -103667,7 +103669,7 @@
         <v>3024</v>
       </c>
       <c r="B30" t="s">
-        <v>3152</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -103675,7 +103677,7 @@
         <v>3025</v>
       </c>
       <c r="B31" t="s">
-        <v>3153</v>
+        <v>3151</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -103683,7 +103685,7 @@
         <v>3026</v>
       </c>
       <c r="B32" t="s">
-        <v>3059</v>
+        <v>3058</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -103691,7 +103693,7 @@
         <v>3027</v>
       </c>
       <c r="B33" t="s">
-        <v>3058</v>
+        <v>3057</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -103699,7 +103701,7 @@
         <v>3028</v>
       </c>
       <c r="B34" t="s">
-        <v>3060</v>
+        <v>3059</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -103707,7 +103709,7 @@
         <v>3029</v>
       </c>
       <c r="B35" t="s">
-        <v>3061</v>
+        <v>3060</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -103715,7 +103717,7 @@
         <v>3030</v>
       </c>
       <c r="B36" t="s">
-        <v>3062</v>
+        <v>3061</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -103723,55 +103725,55 @@
         <v>3031</v>
       </c>
       <c r="B37" t="s">
-        <v>3063</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>3032</v>
+        <v>3157</v>
       </c>
       <c r="B38" t="s">
-        <v>3064</v>
+        <v>3158</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>3150</v>
+        <v>3148</v>
       </c>
       <c r="B39" t="s">
-        <v>3065</v>
+        <v>3063</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>3151</v>
+        <v>3149</v>
       </c>
       <c r="B40" t="s">
-        <v>3066</v>
+        <v>3064</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>3033</v>
+        <v>3032</v>
       </c>
       <c r="B41" t="s">
-        <v>3067</v>
+        <v>3065</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>3034</v>
+        <v>3033</v>
       </c>
       <c r="B42" t="s">
-        <v>3068</v>
+        <v>3066</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>3035</v>
+        <v>3034</v>
       </c>
       <c r="B43" t="s">
-        <v>3069</v>
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -103784,8 +103786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -103795,15 +103797,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3155</v>
+        <v>3153</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>3035</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3036</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3037</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -103811,31 +103813,31 @@
         <v>2775</v>
       </c>
       <c r="B4" t="s">
-        <v>3040</v>
+        <v>3039</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3118</v>
+        <v>3116</v>
       </c>
       <c r="B5" t="s">
-        <v>3124</v>
+        <v>3122</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3070</v>
+        <v>3068</v>
       </c>
       <c r="B6" t="s">
-        <v>3038</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3071</v>
+        <v>3069</v>
       </c>
       <c r="B7" t="s">
-        <v>3085</v>
+        <v>3083</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -103843,7 +103845,7 @@
         <v>2778</v>
       </c>
       <c r="B8" t="s">
-        <v>3086</v>
+        <v>3084</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -103851,79 +103853,79 @@
         <v>2781</v>
       </c>
       <c r="B9" t="s">
-        <v>3157</v>
+        <v>3155</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>3072</v>
+        <v>3070</v>
       </c>
       <c r="B10" t="s">
-        <v>3087</v>
+        <v>3085</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>3073</v>
+        <v>3071</v>
       </c>
       <c r="B11" t="s">
-        <v>3088</v>
+        <v>3086</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>3074</v>
+        <v>3072</v>
       </c>
       <c r="B12" t="s">
-        <v>3089</v>
+        <v>3087</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>3075</v>
+        <v>3073</v>
       </c>
       <c r="B13" t="s">
-        <v>3090</v>
+        <v>3088</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>3076</v>
+        <v>3074</v>
       </c>
       <c r="B14" t="s">
-        <v>3091</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>3119</v>
+        <v>3117</v>
       </c>
       <c r="B15" t="s">
-        <v>3125</v>
+        <v>3123</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>3120</v>
+        <v>3118</v>
       </c>
       <c r="B16" t="s">
-        <v>3126</v>
+        <v>3124</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>3130</v>
+        <v>3128</v>
       </c>
       <c r="B17" t="s">
-        <v>3137</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>3092</v>
+        <v>3090</v>
       </c>
       <c r="B18" t="s">
-        <v>3093</v>
+        <v>3091</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -103939,7 +103941,7 @@
         <v>3019</v>
       </c>
       <c r="B20" t="s">
-        <v>3046</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -103947,223 +103949,223 @@
         <v>3020</v>
       </c>
       <c r="B21" t="s">
-        <v>3054</v>
+        <v>3053</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>3077</v>
+        <v>3075</v>
       </c>
       <c r="B22" t="s">
-        <v>3096</v>
+        <v>3094</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>3121</v>
+        <v>3119</v>
       </c>
       <c r="B23" t="s">
-        <v>3127</v>
+        <v>3125</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>3078</v>
+        <v>3076</v>
       </c>
       <c r="B24" t="s">
-        <v>3097</v>
+        <v>3095</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>3144</v>
+        <v>3142</v>
       </c>
       <c r="B25" t="s">
-        <v>3145</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>3079</v>
+        <v>3077</v>
       </c>
       <c r="B26" t="s">
-        <v>3098</v>
+        <v>3096</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>3080</v>
+        <v>3078</v>
       </c>
       <c r="B27" t="s">
-        <v>3099</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>3081</v>
+        <v>3079</v>
       </c>
       <c r="B28" t="s">
-        <v>3100</v>
+        <v>3098</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>3122</v>
+        <v>3120</v>
       </c>
       <c r="B29" t="s">
-        <v>3128</v>
+        <v>3126</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
       <c r="B30" t="s">
-        <v>3101</v>
+        <v>3099</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>3083</v>
+        <v>3081</v>
       </c>
       <c r="B31" t="s">
-        <v>3102</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>3084</v>
+        <v>3082</v>
       </c>
       <c r="B32" t="s">
-        <v>3103</v>
+        <v>3101</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>3123</v>
+        <v>3121</v>
       </c>
       <c r="B33" t="s">
-        <v>3129</v>
+        <v>3127</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B34" t="s">
         <v>3156</v>
-      </c>
-      <c r="B34" t="s">
-        <v>3158</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>3131</v>
+        <v>3129</v>
       </c>
       <c r="B35" t="s">
-        <v>3138</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>3132</v>
+        <v>3130</v>
       </c>
       <c r="B36" t="s">
-        <v>3140</v>
+        <v>3138</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>3106</v>
+        <v>3104</v>
       </c>
       <c r="B37" t="s">
-        <v>3110</v>
+        <v>3108</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>3107</v>
+        <v>3105</v>
       </c>
       <c r="B38" t="s">
-        <v>3111</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>3112</v>
+      </c>
+      <c r="B39" t="s">
         <v>3114</v>
-      </c>
-      <c r="B39" t="s">
-        <v>3116</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>3113</v>
+      </c>
+      <c r="B40" t="s">
         <v>3115</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3117</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>3133</v>
+        <v>3131</v>
       </c>
       <c r="B41" t="s">
-        <v>3139</v>
+        <v>3137</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>3134</v>
+        <v>3132</v>
       </c>
       <c r="B42" t="s">
-        <v>3141</v>
+        <v>3139</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>3135</v>
+        <v>3133</v>
       </c>
       <c r="B43" t="s">
-        <v>3142</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>3136</v>
+        <v>3134</v>
       </c>
       <c r="B44" t="s">
-        <v>3143</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>3034</v>
+        <v>3033</v>
       </c>
       <c r="B45" t="s">
-        <v>3094</v>
+        <v>3092</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>3035</v>
+        <v>3034</v>
       </c>
       <c r="B46" t="s">
-        <v>3095</v>
+        <v>3093</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>3144</v>
+      </c>
+      <c r="B47" t="s">
         <v>3146</v>
-      </c>
-      <c r="B47" t="s">
-        <v>3148</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>3145</v>
+      </c>
+      <c r="B48" t="s">
         <v>3147</v>
-      </c>
-      <c r="B48" t="s">
-        <v>3149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcting error in transformations to % change/yr and adding column to site year data to detect sites where non-natives were detected
</commit_message>
<xml_diff>
--- a/AquaticMacroInvert_metadata.xlsx
+++ b/AquaticMacroInvert_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\aquatic_data\git\EuroAquaticMacroInverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2962F8A-3BB9-4B5A-85FF-6823CF5E3771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00099546-9FD2-45FD-86FB-6A26BA743F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="1956" windowWidth="17592" windowHeight="11724" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12971" uniqueCount="3155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12973" uniqueCount="3158">
   <si>
     <t>Site_ID</t>
   </si>
@@ -9146,24 +9146,12 @@
     <t>code to identify each unique sampling site</t>
   </si>
   <si>
-    <t>site name in orginal source of data</t>
-  </si>
-  <si>
     <t>country in which site is located</t>
   </si>
   <si>
-    <t>River in which site is located</t>
-  </si>
-  <si>
     <t>name of main data contact for the given site</t>
   </si>
   <si>
-    <t>Longitude in decimal degrees</t>
-  </si>
-  <si>
-    <t>Latitude in decimal degrees</t>
-  </si>
-  <si>
     <t>sampling method description</t>
   </si>
   <si>
@@ -9182,18 +9170,6 @@
     <t>number of years with sampling</t>
   </si>
   <si>
-    <t>first month of the year in which sampling occured across all sampling years</t>
-  </si>
-  <si>
-    <t>last month of the year in which sampling occured across all sampling years</t>
-  </si>
-  <si>
-    <t>season in which sampling occured</t>
-  </si>
-  <si>
-    <t>Primary taxonomic resolution of samples, categorical as Family, genus, or species level</t>
-  </si>
-  <si>
     <t>the number of species in the year with the most species</t>
   </si>
   <si>
@@ -9224,12 +9200,6 @@
     <t>the sum of number of connected dams weighted by distance from sampling site (sum of (100-each dam's distance from site in km)/100) only for dams within 100km of site by river network distance</t>
   </si>
   <si>
-    <t>mean of annual precipitation (mm) across the sampling duration, year was considered as the 12 month periods proceeding the average month of sampling (e.g. for a site with most sampling ocring in May, year was defined as the proceeding May until April)</t>
-  </si>
-  <si>
-    <t>mean of annual maximum temperature (°C) across the sampling duration, year was considered as the 12 month periods proceeding the average month of sampling (e.g. for a site with most sampling ocring in May, year was defined as the proceeding May until April)</t>
-  </si>
-  <si>
     <t>site_id</t>
   </si>
   <si>
@@ -9293,21 +9263,9 @@
     <t>month of sampling</t>
   </si>
   <si>
-    <t>year, with Nas for years with no sampling</t>
-  </si>
-  <si>
     <t>country_wMissing</t>
   </si>
   <si>
-    <t>country in which site is located, with Nas for years with no sampling</t>
-  </si>
-  <si>
-    <t>precipitation (mm) across the sampling duration, year was considered as the 12 month periods proceeding the average month of sampling (e.g. for a site with most sampling ocring in May, year was defined as the proceeding May until April)</t>
-  </si>
-  <si>
-    <t>maximum temperature (°C) across the sampling duration, year was considered as the 12 month periods proceeding the average month of sampling (e.g. for a site with most sampling ocring in May, year was defined as the proceeding May until April)</t>
-  </si>
-  <si>
     <t>number of taxa</t>
   </si>
   <si>
@@ -9317,12 +9275,6 @@
     <t>sum of individuals</t>
   </si>
   <si>
-    <t>temporal turnover (proportion spp gained and lost from codyn R package)</t>
-  </si>
-  <si>
-    <t>functional temporal turnover (proportion spp gained and lost from codyn R package, using functional community weighted means as the "species")</t>
-  </si>
-  <si>
     <t>functional evenness</t>
   </si>
   <si>
@@ -9344,18 +9296,9 @@
     <t>SppRichProportion_alienSpp</t>
   </si>
   <si>
-    <t>Abundance of non-native species; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
-  </si>
-  <si>
     <t>number of non-native species; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
   </si>
   <si>
-    <t>Abundance of non-native species divided by total abundance; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
-  </si>
-  <si>
-    <t>Number of non-native species divided by total abundance; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
-  </si>
-  <si>
     <t>total_abund_AllYrs</t>
   </si>
   <si>
@@ -9368,9 +9311,6 @@
     <t>SppRich_nativeSpp</t>
   </si>
   <si>
-    <t>Abundance of native species; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
-  </si>
-  <si>
     <t>number of native species; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
   </si>
   <si>
@@ -9431,9 +9371,6 @@
     <t>insect_Abund</t>
   </si>
   <si>
-    <t>site ID and year, with Nas for years with no sampling</t>
-  </si>
-  <si>
     <t>number of alien taxa</t>
   </si>
   <si>
@@ -9473,30 +9410,6 @@
     <t>slope of precipitation (mm) over time</t>
   </si>
   <si>
-    <r>
-      <t>slope of maximum temperature (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>⁰C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) over time</t>
-    </r>
-  </si>
-  <si>
     <t>Metadata for variables in the file "All_siteLevel.csv"</t>
   </si>
   <si>
@@ -9516,13 +9429,88 @@
   </si>
   <si>
     <t>mean slope (downstream elevation difference divided by distance) within microbasin site is located (%)</t>
+  </si>
+  <si>
+    <t>alien_detected</t>
+  </si>
+  <si>
+    <t>identifies the 898 sites with species- mixed taxonomic resolution and non-native taxa detected</t>
+  </si>
+  <si>
+    <t>code for unique study in which sites are nested, where study is defined a unique project where samples within have a standardized sampling method and taxonomic resolution</t>
+  </si>
+  <si>
+    <t>site name in original source of data</t>
+  </si>
+  <si>
+    <t>river in which site is located</t>
+  </si>
+  <si>
+    <t>longitude in decimal degrees</t>
+  </si>
+  <si>
+    <t>latitude in decimal degrees</t>
+  </si>
+  <si>
+    <t>first month of the year in which sampling occurred across all sampling years</t>
+  </si>
+  <si>
+    <t>last month of the year in which sampling occurred across all sampling years</t>
+  </si>
+  <si>
+    <t>season in which sampling occurred</t>
+  </si>
+  <si>
+    <t>primary taxonomic resolution of samples, categorical as Family, genus, or species level</t>
+  </si>
+  <si>
+    <t>abundance of non-native species; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
+  </si>
+  <si>
+    <t>abundance of non-native species divided by total abundance; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
+  </si>
+  <si>
+    <t>number of non-native species divided by total abundance; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
+  </si>
+  <si>
+    <t>slope of maximum temperature (⁰C) over time</t>
+  </si>
+  <si>
+    <t>mean of annual precipitation (mm) across the sampling duration, year was considered as the 12 month periods proceeding the average month of sampling (e.g. for a site with most sampling occurring in May, year was defined as the proceeding May until April)</t>
+  </si>
+  <si>
+    <t>mean of annual maximum temperature (°C) across the sampling duration, year was considered as the 12 month periods proceeding the average month of sampling (e.g. for a site with most sampling occurring in May, year was defined as the proceeding May until April)</t>
+  </si>
+  <si>
+    <t>year, with NAs for years with no sampling</t>
+  </si>
+  <si>
+    <t>site ID and year, with NAs for years with no sampling</t>
+  </si>
+  <si>
+    <t>country in which site is located, with NAs for years with no sampling</t>
+  </si>
+  <si>
+    <t>temporal turnover (proportion species gained and lost from codyn R package)</t>
+  </si>
+  <si>
+    <t>functional temporal turnover (proportion species gained and lost from codyn R package, using functional community weighted means as the "species")</t>
+  </si>
+  <si>
+    <t>abundance of native species; NA for sites with family-level taxonomic resolution and likely underestimates non-natives in sites IDed to genus level</t>
+  </si>
+  <si>
+    <t>precipitation (mm) across the sampling duration, year was considered as the 12 month periods proceeding the average month of sampling (e.g. for a site with most sampling occurring in May, year was defined as the proceeding May until April)</t>
+  </si>
+  <si>
+    <t>maximum temperature (°C) across the sampling duration, year was considered as the 12 month periods proceeding the average month of sampling (e.g. for a site with most sampling occurring in May, year was defined as the proceeding May until April)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9842,12 +9830,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -10243,7 +10225,7 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10281,6 +10263,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="36"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="94">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -103422,8 +103414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -103433,7 +103425,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3148</v>
+        <v>3126</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -103445,323 +103437,323 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="17" t="s">
         <v>3017</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="18" t="s">
         <v>3037</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3114</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3120</v>
+      <c r="A5" s="17" t="s">
+        <v>3094</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>3135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="18" t="s">
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>3038</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>3137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>2788</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>3039</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>3138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>3139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>3040</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>2788</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>3041</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>3042</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>3043</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3018</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>3044</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>3019</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>3045</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>2779</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>3140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>2780</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>3141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>2781</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>3142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>3020</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>3143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>3084</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>3085</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>3086</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>3145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>3087</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>3046</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>3022</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>3047</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>3023</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>3048</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="17" t="s">
+        <v>3089</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
+        <v>3024</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>3025</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>3147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
+        <v>3026</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
+        <v>3027</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>3049</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>2779</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3050</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>2780</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="17" t="s">
+        <v>3028</v>
+      </c>
+      <c r="B34" s="18" t="s">
         <v>3051</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>2781</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="17" t="s">
+        <v>3029</v>
+      </c>
+      <c r="B35" s="18" t="s">
         <v>3052</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>3020</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="17" t="s">
+        <v>3030</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>3053</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>3100</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>3101</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>3102</v>
-      </c>
-      <c r="B24" t="s">
-        <v>3106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>3103</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>3021</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="17" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>3054</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>3022</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="17" t="s">
+        <v>3131</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>3132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
+        <v>3121</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="17" t="s">
+        <v>3122</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>3124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
+        <v>3032</v>
+      </c>
+      <c r="B41" s="18" t="s">
         <v>3055</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>3023</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3056</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>3108</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>3024</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>3025</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>3026</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3058</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>3027</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3057</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>3028</v>
-      </c>
-      <c r="B34" t="s">
-        <v>3059</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>3029</v>
-      </c>
-      <c r="B35" t="s">
-        <v>3060</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>3030</v>
-      </c>
-      <c r="B36" t="s">
-        <v>3061</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>3031</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3062</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>3153</v>
-      </c>
-      <c r="B38" t="s">
-        <v>3154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>3142</v>
-      </c>
-      <c r="B39" t="s">
-        <v>3144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>3143</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>3032</v>
-      </c>
-      <c r="B41" t="s">
-        <v>3063</v>
-      </c>
-    </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="17" t="s">
         <v>3033</v>
       </c>
-      <c r="B42" t="s">
-        <v>3064</v>
+      <c r="B42" s="18" t="s">
+        <v>3148</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="17" t="s">
         <v>3034</v>
       </c>
-      <c r="B43" t="s">
-        <v>3065</v>
+      <c r="B43" s="18" t="s">
+        <v>3149</v>
       </c>
     </row>
   </sheetData>
@@ -103772,388 +103764,397 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3149</v>
+        <v>3127</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3035</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="20" t="s">
         <v>3036</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="17" t="s">
         <v>2775</v>
       </c>
-      <c r="B4" t="s">
-        <v>3039</v>
+      <c r="B4" s="21" t="s">
+        <v>3038</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="17" t="s">
+        <v>3094</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>3056</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>3037</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>3057</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>3071</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>2778</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>2781</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>3129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>3058</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>3073</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>3059</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>3074</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>3060</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>3061</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>3076</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>3062</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>3095</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>3101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>3096</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>3102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>3106</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>3077</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>3152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>3041</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>3020</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>3143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>3063</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>3078</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>3097</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>3064</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>3119</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>3065</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>3066</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>3067</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>3154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="17" t="s">
+        <v>3098</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>3104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
+        <v>3068</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>3081</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>3069</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>3082</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
+        <v>3070</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>3083</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
+        <v>3099</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>3105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="17" t="s">
+        <v>3128</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="17" t="s">
+        <v>3107</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>3113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="17" t="s">
+        <v>3108</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>3115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="17" t="s">
+        <v>3133</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>3134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="17" t="s">
+        <v>3086</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>3145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
+        <v>3087</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="17" t="s">
+        <v>3091</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
+        <v>3092</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="17" t="s">
+        <v>3109</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>3114</v>
       </c>
-      <c r="B5" t="s">
-        <v>3120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3066</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3037</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>3067</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3081</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>2778</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3082</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>2781</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>3068</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3083</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>3069</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3084</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3070</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3085</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>3071</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3086</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>3072</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3087</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>3115</v>
-      </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="17" t="s">
+        <v>3110</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>3116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
+        <v>3111</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="17" t="s">
+        <v>3112</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>3118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="17" t="s">
+        <v>3033</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="17" t="s">
+        <v>3034</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>3157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="17" t="s">
         <v>3121</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>3116</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B48" s="21" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
         <v>3122</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>3126</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>3088</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3089</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>3018</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>3019</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3045</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>3020</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3053</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>3073</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>3117</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>3074</v>
-      </c>
-      <c r="B24" t="s">
-        <v>3093</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>3140</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>3075</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3094</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>3076</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3095</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>3077</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3096</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>3118</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="B49" s="21" t="s">
         <v>3124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>3078</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3097</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>3079</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3098</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>3080</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3099</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>3119</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>3150</v>
-      </c>
-      <c r="B34" t="s">
-        <v>3152</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>3127</v>
-      </c>
-      <c r="B35" t="s">
-        <v>3134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>3128</v>
-      </c>
-      <c r="B36" t="s">
-        <v>3136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>3102</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>3103</v>
-      </c>
-      <c r="B38" t="s">
-        <v>3107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>3110</v>
-      </c>
-      <c r="B39" t="s">
-        <v>3112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>3111</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>3129</v>
-      </c>
-      <c r="B41" t="s">
-        <v>3135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>3130</v>
-      </c>
-      <c r="B42" t="s">
-        <v>3137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>3131</v>
-      </c>
-      <c r="B43" t="s">
-        <v>3138</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>3132</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>3033</v>
-      </c>
-      <c r="B45" t="s">
-        <v>3090</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>3034</v>
-      </c>
-      <c r="B46" t="s">
-        <v>3091</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>3142</v>
-      </c>
-      <c r="B47" t="s">
-        <v>3144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>3143</v>
-      </c>
-      <c r="B48" t="s">
-        <v>3145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>